<commit_message>
Structural & visual design done, Gantt chart Done
</commit_message>
<xml_diff>
--- a/Gantt chart.xlsx
+++ b/Gantt chart.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25427"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bfd74915eb265310/Teaching/1810ICT/Assignment/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tieha\Downloads\2810ict\2810ict_Assignment\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19F6BFA9-E389-4EF4-895E-EB7CFE0BA8D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9516"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project Planner" sheetId="1" r:id="rId1"/>
@@ -26,8 +27,18 @@
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Project Planner'!$3:$4</definedName>
     <definedName name="TitleRegion..BO60">'Project Planner'!$B$3:$B$4</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -42,69 +53,6 @@
   </si>
   <si>
     <t>ACTIVITY</t>
-  </si>
-  <si>
-    <t>Activity 01</t>
-  </si>
-  <si>
-    <t>Activity 02</t>
-  </si>
-  <si>
-    <t>Activity 03</t>
-  </si>
-  <si>
-    <t>Activity 04</t>
-  </si>
-  <si>
-    <t>Activity 05</t>
-  </si>
-  <si>
-    <t>Activity 06</t>
-  </si>
-  <si>
-    <t>Activity 07</t>
-  </si>
-  <si>
-    <t>Activity 08</t>
-  </si>
-  <si>
-    <t>Activity 09</t>
-  </si>
-  <si>
-    <t>Activity 10</t>
-  </si>
-  <si>
-    <t>Activity 11</t>
-  </si>
-  <si>
-    <t>Activity 12</t>
-  </si>
-  <si>
-    <t>Activity 13</t>
-  </si>
-  <si>
-    <t>Activity 14</t>
-  </si>
-  <si>
-    <t>Activity 15</t>
-  </si>
-  <si>
-    <t>Activity 16</t>
-  </si>
-  <si>
-    <t>Activity 17</t>
-  </si>
-  <si>
-    <t>Activity 18</t>
-  </si>
-  <si>
-    <t>Activity 19</t>
-  </si>
-  <si>
-    <t>Activity 20</t>
-  </si>
-  <si>
-    <t>Activity 21</t>
   </si>
   <si>
     <t>Activity 22</t>
@@ -257,14 +205,99 @@
     <t>Activity 35</t>
   </si>
   <si>
-    <t>Project Title</t>
+    <t>1.Concept</t>
+    <phoneticPr fontId="14" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1.1Develop project plan</t>
+    <phoneticPr fontId="14" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1.2Define requirements</t>
+    <phoneticPr fontId="14" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">  1.2.1User requirements</t>
+    <phoneticPr fontId="14" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">  1.2.2Software requirements</t>
+    <phoneticPr fontId="14" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">  1.2.3Use Case &amp; Use Case Diagram</t>
+    <phoneticPr fontId="14" type="noConversion"/>
+  </si>
+  <si>
+    <t>2.Design</t>
+    <phoneticPr fontId="14" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2.1Software Design</t>
+    <phoneticPr fontId="14" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2.2Define software components</t>
+    <phoneticPr fontId="14" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">  2.2.1Functions</t>
+    <phoneticPr fontId="14" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">  2.2.2Data structures</t>
+    <phoneticPr fontId="14" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">  2.2.3Detailed Design</t>
+    <phoneticPr fontId="14" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2.3User interface Design</t>
+    <phoneticPr fontId="14" type="noConversion"/>
+  </si>
+  <si>
+    <t>3.Software Development</t>
+    <phoneticPr fontId="14" type="noConversion"/>
+  </si>
+  <si>
+    <t>4.Test</t>
+    <phoneticPr fontId="14" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> 4.1Unit test</t>
+    <phoneticPr fontId="14" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> 4.2Coverage Report</t>
+    <phoneticPr fontId="14" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> 4.3Requirement Acceptance Testing</t>
+    <phoneticPr fontId="14" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> 5.Executive Summary</t>
+    <phoneticPr fontId="14" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">  2.3.1Structural Design</t>
+    <phoneticPr fontId="14" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">  2.3.2 Visual Design</t>
+    <phoneticPr fontId="14" type="noConversion"/>
+  </si>
+  <si>
+    <t>Group 98_2810ICT_2022</t>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="14" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1" tint="0.24994659260841701"/>
@@ -364,8 +397,22 @@
       <family val="2"/>
       <scheme val="major"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="돋움"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="1" tint="0.24994659260841701"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -404,6 +451,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -551,7 +610,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -582,7 +641,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="4" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="4">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -618,12 +677,57 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="11">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" xfId="2" applyFont="1" applyFill="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="2" applyFill="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" xfId="2" applyFont="1" applyFill="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="10" applyBorder="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="10" applyBorder="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="5" applyFont="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="12">
       <alignment vertical="center"/>
     </xf>
@@ -636,178 +740,29 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="10">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="10" applyBorder="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="10" applyBorder="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="5" applyFont="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="19">
-    <cellStyle name="% complete" xfId="16"/>
-    <cellStyle name="% complete (beyond plan) legend" xfId="18"/>
-    <cellStyle name="Activity" xfId="2"/>
-    <cellStyle name="Actual (beyond plan) legend" xfId="17"/>
-    <cellStyle name="Actual legend" xfId="15"/>
-    <cellStyle name="Explanatory Text" xfId="12" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="1" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="9" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="10" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="11" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Label" xfId="5"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
-    <cellStyle name="Percent Complete" xfId="6"/>
-    <cellStyle name="Period Headers" xfId="3"/>
-    <cellStyle name="Period Highlight Control" xfId="7"/>
-    <cellStyle name="Period Value" xfId="13"/>
-    <cellStyle name="Plan legend" xfId="14"/>
-    <cellStyle name="Project Headers" xfId="4"/>
-    <cellStyle name="Title" xfId="8" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="% complete" xfId="16" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="% complete (beyond plan) legend" xfId="18" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Activity" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Actual (beyond plan) legend" xfId="17" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Actual legend" xfId="15" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="Label" xfId="5" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
+    <cellStyle name="Percent Complete" xfId="6" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
+    <cellStyle name="Period Headers" xfId="3" xr:uid="{00000000-0005-0000-0000-00000D000000}"/>
+    <cellStyle name="Period Highlight Control" xfId="7" xr:uid="{00000000-0005-0000-0000-00000E000000}"/>
+    <cellStyle name="Period Value" xfId="13" xr:uid="{00000000-0005-0000-0000-00000F000000}"/>
+    <cellStyle name="Plan legend" xfId="14" xr:uid="{00000000-0005-0000-0000-000010000000}"/>
+    <cellStyle name="Project Headers" xfId="4" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
+    <cellStyle name="설명 텍스트" xfId="12" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="제목" xfId="8" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="제목 1" xfId="1" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="제목 2" xfId="9" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="제목 3" xfId="10" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="제목 4" xfId="11" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="표준" xfId="0" builtinId="0" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="18">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="9" tint="-0.24994659260841701"/>
-        </left>
-        <right style="thin">
-          <color theme="9" tint="-0.24994659260841701"/>
-        </right>
-        <bottom style="thin">
-          <color theme="9" tint="0.59996337778862885"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7"/>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7"/>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
+  <dxfs count="9">
     <dxf>
       <fill>
         <patternFill>
@@ -824,15 +779,6 @@
         <bottom style="thin">
           <color theme="7"/>
         </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <top style="thin">
-          <color theme="7"/>
-        </top>
         <vertical/>
         <horizontal/>
       </border>
@@ -1189,31 +1135,34 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor theme="7"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="B1:BO39"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="AU20" sqref="AU20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="2.77734375" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.6640625" customWidth="1"/>
-    <col min="2" max="2" width="26.33203125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.44140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="27" width="2.77734375" style="1"/>
-    <col min="42" max="42" width="2.77734375" customWidth="1"/>
+    <col min="1" max="1" width="2.625" customWidth="1"/>
+    <col min="2" max="2" width="26.375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="11.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.625" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="3.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="16" width="3.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="27" width="4.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="40" width="4.25" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="2.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:67" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="1.05">
+    <row r="1" spans="2:67" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.85">
       <c r="B1" s="14" t="s">
         <v>49</v>
       </c>
@@ -1223,82 +1172,82 @@
       <c r="F1" s="13"/>
       <c r="G1" s="13"/>
     </row>
-    <row r="2" spans="2:67" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
+    <row r="2" spans="2:67" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="39" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
       <c r="G2" s="5" t="s">
-        <v>31</v>
+        <v>10</v>
       </c>
       <c r="H2" s="15">
         <v>1</v>
       </c>
       <c r="J2" s="16"/>
-      <c r="K2" s="30" t="s">
-        <v>38</v>
-      </c>
-      <c r="L2" s="31"/>
-      <c r="M2" s="31"/>
-      <c r="N2" s="31"/>
-      <c r="O2" s="32"/>
+      <c r="K2" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="L2" s="33"/>
+      <c r="M2" s="33"/>
+      <c r="N2" s="33"/>
+      <c r="O2" s="34"/>
       <c r="P2" s="17"/>
-      <c r="Q2" s="30" t="s">
-        <v>37</v>
-      </c>
-      <c r="R2" s="33"/>
-      <c r="S2" s="33"/>
-      <c r="T2" s="32"/>
+      <c r="Q2" s="32" t="s">
+        <v>16</v>
+      </c>
+      <c r="R2" s="35"/>
+      <c r="S2" s="35"/>
+      <c r="T2" s="34"/>
       <c r="U2" s="18"/>
-      <c r="V2" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="W2" s="23"/>
-      <c r="X2" s="23"/>
-      <c r="Y2" s="34"/>
+      <c r="V2" s="36" t="s">
+        <v>7</v>
+      </c>
+      <c r="W2" s="37"/>
+      <c r="X2" s="37"/>
+      <c r="Y2" s="38"/>
       <c r="Z2" s="19"/>
-      <c r="AA2" s="35" t="s">
-        <v>29</v>
-      </c>
-      <c r="AB2" s="36"/>
-      <c r="AC2" s="36"/>
-      <c r="AD2" s="36"/>
-      <c r="AE2" s="36"/>
-      <c r="AF2" s="36"/>
-      <c r="AG2" s="37"/>
+      <c r="AA2" s="36" t="s">
+        <v>8</v>
+      </c>
+      <c r="AB2" s="37"/>
+      <c r="AC2" s="37"/>
+      <c r="AD2" s="37"/>
+      <c r="AE2" s="37"/>
+      <c r="AF2" s="37"/>
+      <c r="AG2" s="38"/>
       <c r="AH2" s="20"/>
-      <c r="AI2" s="38" t="s">
-        <v>30</v>
-      </c>
-      <c r="AJ2" s="39"/>
-      <c r="AK2" s="39"/>
-      <c r="AL2" s="39"/>
-      <c r="AM2" s="39"/>
-      <c r="AN2" s="39"/>
-      <c r="AO2" s="39"/>
-      <c r="AP2" s="39"/>
-    </row>
-    <row r="3" spans="2:67" s="12" customFormat="1" ht="39.9" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="25" t="s">
+      <c r="AI2" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="AJ2" s="23"/>
+      <c r="AK2" s="23"/>
+      <c r="AL2" s="23"/>
+      <c r="AM2" s="23"/>
+      <c r="AN2" s="23"/>
+      <c r="AO2" s="23"/>
+      <c r="AP2" s="23"/>
+    </row>
+    <row r="3" spans="2:67" s="12" customFormat="1" ht="39.950000000000003" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="27" t="s">
-        <v>32</v>
-      </c>
-      <c r="D3" s="27" t="s">
-        <v>33</v>
-      </c>
-      <c r="E3" s="27" t="s">
-        <v>34</v>
-      </c>
-      <c r="F3" s="27" t="s">
-        <v>35</v>
-      </c>
-      <c r="G3" s="29" t="s">
-        <v>36</v>
+      <c r="C3" s="42" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="42" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="42" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="42" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="30" t="s">
+        <v>15</v>
       </c>
       <c r="H3" s="21" t="s">
         <v>0</v>
@@ -1323,13 +1272,13 @@
       <c r="Z3" s="11"/>
       <c r="AA3" s="11"/>
     </row>
-    <row r="4" spans="2:67" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="26"/>
-      <c r="C4" s="28"/>
-      <c r="D4" s="28"/>
-      <c r="E4" s="28"/>
-      <c r="F4" s="28"/>
-      <c r="G4" s="28"/>
+    <row r="4" spans="2:67" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="41"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="31"/>
+      <c r="G4" s="31"/>
       <c r="H4" s="3">
         <v>1</v>
       </c>
@@ -1511,265 +1460,341 @@
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="6" t="s">
+    <row r="5" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="25"/>
+      <c r="D5" s="25"/>
+      <c r="E5" s="25"/>
+      <c r="F5" s="25"/>
+      <c r="G5" s="25"/>
+    </row>
+    <row r="6" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" s="7">
+        <v>1</v>
+      </c>
+      <c r="D6" s="7">
+        <v>4</v>
+      </c>
+      <c r="E6" s="7">
+        <v>1</v>
+      </c>
+      <c r="F6" s="7">
+        <v>5</v>
+      </c>
+      <c r="G6" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" s="29"/>
+      <c r="D7" s="29"/>
+      <c r="E7" s="29"/>
+      <c r="F7" s="29"/>
+      <c r="G7" s="29"/>
+    </row>
+    <row r="8" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="7">
+        <v>4</v>
+      </c>
+      <c r="D8" s="7">
+        <v>3</v>
+      </c>
+      <c r="E8" s="7">
+        <v>11</v>
+      </c>
+      <c r="F8" s="7">
+        <v>11</v>
+      </c>
+      <c r="G8" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="2:67" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" s="7">
+        <v>7</v>
+      </c>
+      <c r="D9" s="7">
+        <v>5</v>
+      </c>
+      <c r="E9" s="7">
+        <v>16</v>
+      </c>
+      <c r="F9" s="7">
+        <v>6</v>
+      </c>
+      <c r="G9" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="2:67" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" s="7">
+        <v>11</v>
+      </c>
+      <c r="D10" s="7">
         <v>2</v>
       </c>
-      <c r="C5" s="7">
+      <c r="E10" s="7">
+        <v>21</v>
+      </c>
+      <c r="F10" s="7">
+        <v>2</v>
+      </c>
+      <c r="G10" s="8">
         <v>1</v>
       </c>
-      <c r="D5" s="7">
+    </row>
+    <row r="11" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" s="25"/>
+      <c r="D11" s="25"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="25"/>
+      <c r="G11" s="25"/>
+    </row>
+    <row r="12" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" s="7">
+        <v>14</v>
+      </c>
+      <c r="D12" s="7">
+        <v>2</v>
+      </c>
+      <c r="E12" s="7">
+        <v>21</v>
+      </c>
+      <c r="F12" s="7">
+        <v>2</v>
+      </c>
+      <c r="G12" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="2:67" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" s="29"/>
+      <c r="D13" s="29"/>
+      <c r="E13" s="29"/>
+      <c r="F13" s="29"/>
+      <c r="G13" s="29"/>
+    </row>
+    <row r="14" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14" s="7">
+        <v>16</v>
+      </c>
+      <c r="D14" s="7">
         <v>5</v>
       </c>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="6" t="s">
+      <c r="E14" s="7">
+        <v>22</v>
+      </c>
+      <c r="F14" s="7">
+        <v>2</v>
+      </c>
+      <c r="G14" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="C15" s="9">
+        <v>18</v>
+      </c>
+      <c r="D15" s="7">
+        <v>6</v>
+      </c>
+      <c r="E15" s="7">
+        <v>23</v>
+      </c>
+      <c r="F15" s="7">
         <v>3</v>
       </c>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="6" t="s">
+      <c r="G15" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16" s="7">
+        <v>24</v>
+      </c>
+      <c r="D16" s="7">
+        <v>2</v>
+      </c>
+      <c r="E16" s="7">
+        <v>24</v>
+      </c>
+      <c r="F16" s="7">
+        <v>2</v>
+      </c>
+      <c r="G16" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="28" t="s">
+        <v>40</v>
+      </c>
+      <c r="C17" s="29"/>
+      <c r="D17" s="29"/>
+      <c r="E17" s="29"/>
+      <c r="F17" s="29"/>
+      <c r="G17" s="29"/>
+    </row>
+    <row r="18" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C18" s="7">
+        <v>24</v>
+      </c>
+      <c r="D18" s="7">
         <v>4</v>
       </c>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C15" s="9"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
-      <c r="G17" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C18" s="7"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
+      <c r="E18" s="7">
+        <v>25</v>
+      </c>
+      <c r="F18" s="7">
+        <v>2</v>
+      </c>
       <c r="G18" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B19" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="24" t="s">
+        <v>48</v>
+      </c>
+      <c r="C19" s="7">
+        <v>25</v>
+      </c>
+      <c r="D19" s="7">
+        <v>3</v>
+      </c>
+      <c r="E19" s="7">
+        <v>26</v>
+      </c>
+      <c r="F19" s="7">
+        <v>2</v>
+      </c>
       <c r="G19" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B20" s="6" t="s">
-        <v>17</v>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="24" t="s">
+        <v>41</v>
       </c>
       <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
+      <c r="D20" s="7">
+        <v>28</v>
+      </c>
       <c r="E20" s="7"/>
       <c r="F20" s="7"/>
       <c r="G20" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B21" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C21" s="7"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="7"/>
-      <c r="F21" s="7"/>
+    <row r="21" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="C21" s="25"/>
+      <c r="D21" s="25"/>
+      <c r="E21" s="25"/>
+      <c r="F21" s="25"/>
       <c r="G21" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B22" s="6" t="s">
-        <v>19</v>
+    <row r="22" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="24" t="s">
+        <v>43</v>
       </c>
       <c r="C22" s="7"/>
-      <c r="D22" s="7"/>
+      <c r="D22" s="7">
+        <v>7</v>
+      </c>
       <c r="E22" s="7"/>
       <c r="F22" s="7"/>
       <c r="G22" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B23" s="6" t="s">
-        <v>20</v>
+    <row r="23" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="24" t="s">
+        <v>44</v>
       </c>
       <c r="C23" s="7"/>
-      <c r="D23" s="7"/>
+      <c r="D23" s="7">
+        <v>5</v>
+      </c>
       <c r="E23" s="7"/>
       <c r="F23" s="7"/>
       <c r="G23" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B24" s="6" t="s">
-        <v>21</v>
+    <row r="24" spans="2:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="24" t="s">
+        <v>45</v>
       </c>
       <c r="C24" s="7"/>
-      <c r="D24" s="7"/>
+      <c r="D24" s="7">
+        <v>5</v>
+      </c>
       <c r="E24" s="7"/>
       <c r="F24" s="7"/>
       <c r="G24" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B25" s="6" t="s">
-        <v>22</v>
+    <row r="25" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="24" t="s">
+        <v>46</v>
       </c>
       <c r="C25" s="7"/>
-      <c r="D25" s="7"/>
+      <c r="D25" s="7">
+        <v>6</v>
+      </c>
       <c r="E25" s="7"/>
       <c r="F25" s="7"/>
       <c r="G25" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B26" s="6" t="s">
-        <v>23</v>
+        <v>2</v>
       </c>
       <c r="C26" s="7"/>
       <c r="D26" s="7"/>
@@ -1779,9 +1804,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B27" s="6" t="s">
-        <v>24</v>
+        <v>3</v>
       </c>
       <c r="C27" s="7"/>
       <c r="D27" s="7"/>
@@ -1791,9 +1816,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B28" s="6" t="s">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="C28" s="7"/>
       <c r="D28" s="7"/>
@@ -1803,9 +1828,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B29" s="6" t="s">
-        <v>26</v>
+        <v>5</v>
       </c>
       <c r="C29" s="7"/>
       <c r="D29" s="7"/>
@@ -1815,9 +1840,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B30" s="6" t="s">
-        <v>27</v>
+        <v>6</v>
       </c>
       <c r="C30" s="7"/>
       <c r="D30" s="7"/>
@@ -1827,9 +1852,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B31" s="6" t="s">
-        <v>40</v>
+        <v>19</v>
       </c>
       <c r="C31" s="7"/>
       <c r="D31" s="7"/>
@@ -1839,9 +1864,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B32" s="6" t="s">
-        <v>41</v>
+        <v>20</v>
       </c>
       <c r="C32" s="7"/>
       <c r="D32" s="7"/>
@@ -1851,9 +1876,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B33" s="6" t="s">
-        <v>42</v>
+        <v>21</v>
       </c>
       <c r="C33" s="7"/>
       <c r="D33" s="7"/>
@@ -1863,9 +1888,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B34" s="6" t="s">
-        <v>43</v>
+        <v>22</v>
       </c>
       <c r="C34" s="7"/>
       <c r="D34" s="7"/>
@@ -1875,9 +1900,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B35" s="6" t="s">
-        <v>44</v>
+        <v>23</v>
       </c>
       <c r="C35" s="7"/>
       <c r="D35" s="7"/>
@@ -1887,9 +1912,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B36" s="6" t="s">
-        <v>45</v>
+        <v>24</v>
       </c>
       <c r="C36" s="7"/>
       <c r="D36" s="7"/>
@@ -1899,9 +1924,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B37" s="6" t="s">
-        <v>46</v>
+        <v>25</v>
       </c>
       <c r="C37" s="7"/>
       <c r="D37" s="7"/>
@@ -1911,9 +1936,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B38" s="6" t="s">
-        <v>47</v>
+        <v>26</v>
       </c>
       <c r="C38" s="7"/>
       <c r="D38" s="7"/>
@@ -1923,9 +1948,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B39" s="6" t="s">
-        <v>48</v>
+        <v>27</v>
       </c>
       <c r="C39" s="7"/>
       <c r="D39" s="7"/>
@@ -1949,60 +1974,61 @@
     <mergeCell ref="V2:Y2"/>
     <mergeCell ref="AA2:AG2"/>
   </mergeCells>
+  <phoneticPr fontId="14" type="noConversion"/>
   <conditionalFormatting sqref="H5:BO39">
-    <cfRule type="expression" dxfId="17" priority="1">
+    <cfRule type="expression" dxfId="8" priority="1">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="3">
+    <cfRule type="expression" dxfId="7" priority="3">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="15" priority="4">
+    <cfRule type="expression" dxfId="6" priority="4">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="5">
+    <cfRule type="expression" dxfId="5" priority="5">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="6">
+    <cfRule type="expression" dxfId="4" priority="6">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="7">
+    <cfRule type="expression" dxfId="3" priority="7">
       <formula>H$4=period_selected</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="11">
+    <cfRule type="expression" dxfId="2" priority="11">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="12">
+    <cfRule type="expression" dxfId="1" priority="12">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4:BO4">
-    <cfRule type="expression" dxfId="8" priority="8">
+    <cfRule type="expression" dxfId="0" priority="8">
       <formula>H$4=period_selected</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="16">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Project planner uses periods for intervals. Start=1 is period 1 and duration=5 means project spans 5 periods starting from start period. Enter data starting in B5 to update the chart" sqref="A1"/>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Type a value from 1 to 60 or select a period from the list-press  CANCEL, ALT+DOWN ARROW, then ENTER to select a value" prompt="Enter a period in the range of 1 to 60 or select a period from the list. Press ALT+DOWN ARROW to navigate the list, then ENTER to select a value" sqref="H2">
+  <dataValidations disablePrompts="1" count="16">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Project planner uses periods for intervals. Start=1 is period 1 and duration=5 means project spans 5 periods starting from start period. Enter data starting in B5 to update the chart" sqref="A1" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Type a value from 1 to 60 or select a period from the list-press  CANCEL, ALT+DOWN ARROW, then ENTER to select a value" prompt="Enter a period in the range of 1 to 60 or select a period from the list. Press ALT+DOWN ARROW to navigate the list, then ENTER to select a value" sqref="H2" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"1,2,3,4,5,6,7,8,9,10,11,12,13,14,15,16,17,18,19,20,21,22,23,24,25,26,27,28,29,30,31,32,33,34,35,36,37,38,39,40,41,42,43,44,45,46,47,48,49,50,51,52,53,54,55,56,57,58,59,60"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates plan duration" sqref="J2"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates actual duration" sqref="P2"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates the percentage of project completed" sqref="U2"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates actual duration beyond plan" sqref="Z2"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates the percentage of project completed beyond plan" sqref="AH2"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Periods are charted from 1 to 60 starting from cell H4 to cell BO4 " sqref="H3"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter activity in column B, starting with cell B5_x000a_" sqref="B3:B4"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter plan start period in column C, starting with cell C5" sqref="C3:C4"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter plan duration period in column D, starting with cell D5" sqref="D3:D4"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter actual start period in column E, starting with cell E5" sqref="E3:E4"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter actual duration period in column F, starting with cell F5" sqref="F3:F4"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter the percentage of project completed in column G, starting with cell G5" sqref="G3:G4"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Title of the project. Enter a new title in this cell. Highlight a period in H2. Chart legend is in J2 to AI2" sqref="B1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Select a period to highlight in H2. A Chart legend is in J2 to AI2" sqref="B2:F2"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates plan duration" sqref="J2" xr:uid="{00000000-0002-0000-0000-000002000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates actual duration" sqref="P2" xr:uid="{00000000-0002-0000-0000-000003000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates the percentage of project completed" sqref="U2" xr:uid="{00000000-0002-0000-0000-000004000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates actual duration beyond plan" sqref="Z2" xr:uid="{00000000-0002-0000-0000-000005000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates the percentage of project completed beyond plan" sqref="AH2" xr:uid="{00000000-0002-0000-0000-000006000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Periods are charted from 1 to 60 starting from cell H4 to cell BO4 " sqref="H3" xr:uid="{00000000-0002-0000-0000-000007000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter activity in column B, starting with cell B5_x000a_" sqref="B3:B4" xr:uid="{00000000-0002-0000-0000-000008000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter plan start period in column C, starting with cell C5" sqref="C3:C4" xr:uid="{00000000-0002-0000-0000-000009000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter plan duration period in column D, starting with cell D5" sqref="D3:D4" xr:uid="{00000000-0002-0000-0000-00000A000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter actual start period in column E, starting with cell E5" sqref="E3:E4" xr:uid="{00000000-0002-0000-0000-00000B000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter actual duration period in column F, starting with cell F5" sqref="F3:F4" xr:uid="{00000000-0002-0000-0000-00000C000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter the percentage of project completed in column G, starting with cell G5" sqref="G3:G4" xr:uid="{00000000-0002-0000-0000-00000D000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Title of the project. Enter a new title in this cell. Highlight a period in H2. Chart legend is in J2 to AI2" sqref="B1" xr:uid="{00000000-0002-0000-0000-00000E000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Select a period to highlight in H2. A Chart legend is in J2 to AI2" sqref="B2:F2" xr:uid="{00000000-0002-0000-0000-00000F000000}"/>
   </dataValidations>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.45" right="0.45" top="0.5" bottom="0.5" header="0.3" footer="0.3"/>
-  <pageSetup scale="51" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <pageSetup scale="45" fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <headerFooter differentFirst="1">
     <oddFooter>Page &amp;P of &amp;N</oddFooter>
   </headerFooter>

</xml_diff>

<commit_message>
Gantt chart updated and attached into Project plan, Proofread of other docx
</commit_message>
<xml_diff>
--- a/Gantt chart.xlsx
+++ b/Gantt chart.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25629"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tieha\Downloads\2810ict\2810ict_Assignment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19F6BFA9-E389-4EF4-895E-EB7CFE0BA8D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23DBC9E4-D076-419F-A2F6-929CC3CB4C96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Project Planner" sheetId="1" r:id="rId1"/>
+    <sheet name="Chart1" sheetId="2" state="hidden" r:id="rId1"/>
+    <sheet name="Project Planner" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="Actual">(PeriodInActual*('Project Planner'!$E1&gt;0))*PeriodInPlan</definedName>
@@ -24,7 +25,7 @@
     <definedName name="PeriodInActual">'Project Planner'!A$4=MEDIAN('Project Planner'!A$4,'Project Planner'!$E1,'Project Planner'!$E1+'Project Planner'!$F1-1)</definedName>
     <definedName name="PeriodInPlan">'Project Planner'!A$4=MEDIAN('Project Planner'!A$4,'Project Planner'!$C1,'Project Planner'!$C1+'Project Planner'!$D1-1)</definedName>
     <definedName name="Plan">PeriodInPlan*('Project Planner'!$C1&gt;0)</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="0">'Project Planner'!$3:$4</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="1">'Project Planner'!$3:$4</definedName>
     <definedName name="TitleRegion..BO60">'Project Planner'!$B$3:$B$4</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -53,9 +54,6 @@
   </si>
   <si>
     <t>ACTIVITY</t>
-  </si>
-  <si>
-    <t>Activity 22</t>
   </si>
   <si>
     <t>Activity 23</t>
@@ -290,6 +288,10 @@
   </si>
   <si>
     <t>Group 98_2810ICT_2022</t>
+    <phoneticPr fontId="14" type="noConversion"/>
+  </si>
+  <si>
+    <t>6.User guide for program</t>
     <phoneticPr fontId="14" type="noConversion"/>
   </si>
 </sst>
@@ -701,12 +703,24 @@
     <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="12">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="9">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="9" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="10">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="10" applyBorder="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="10" applyBorder="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="10" applyBorder="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -727,18 +741,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="12">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="9">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="9" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="10">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="19">
@@ -907,6 +909,809 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="ko-KR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ko-KR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="544585871"/>
+        <c:axId val="811976895"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="544585871"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ko-KR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="811976895"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="811976895"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ko-KR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="544585871"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="ko-KR"/>
+    </a:p>
+  </c:txPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{C44A68F1-292B-4A72-AEEF-152D4F05207A}">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView zoomScale="97" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="9299149" cy="6078325"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="차트 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{981B4A59-0B8C-B640-7B07-C9D939502373}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1142,8 +1947,8 @@
   </sheetPr>
   <dimension ref="B1:BO39"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="AU20" sqref="AU20"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" zoomScale="55" zoomScaleNormal="55" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="AK28" sqref="AK28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1164,7 +1969,7 @@
   <sheetData>
     <row r="1" spans="2:67" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.85">
       <c r="B1" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C1" s="13"/>
       <c r="D1" s="13"/>
@@ -1173,54 +1978,54 @@
       <c r="G1" s="13"/>
     </row>
     <row r="2" spans="2:67" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="39" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
+      <c r="B2" s="30" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
       <c r="G2" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H2" s="15">
         <v>1</v>
       </c>
       <c r="J2" s="16"/>
-      <c r="K2" s="32" t="s">
-        <v>17</v>
-      </c>
-      <c r="L2" s="33"/>
-      <c r="M2" s="33"/>
-      <c r="N2" s="33"/>
-      <c r="O2" s="34"/>
+      <c r="K2" s="36" t="s">
+        <v>16</v>
+      </c>
+      <c r="L2" s="37"/>
+      <c r="M2" s="37"/>
+      <c r="N2" s="37"/>
+      <c r="O2" s="38"/>
       <c r="P2" s="17"/>
-      <c r="Q2" s="32" t="s">
-        <v>16</v>
-      </c>
-      <c r="R2" s="35"/>
-      <c r="S2" s="35"/>
-      <c r="T2" s="34"/>
+      <c r="Q2" s="36" t="s">
+        <v>15</v>
+      </c>
+      <c r="R2" s="39"/>
+      <c r="S2" s="39"/>
+      <c r="T2" s="38"/>
       <c r="U2" s="18"/>
-      <c r="V2" s="36" t="s">
+      <c r="V2" s="40" t="s">
+        <v>6</v>
+      </c>
+      <c r="W2" s="41"/>
+      <c r="X2" s="41"/>
+      <c r="Y2" s="42"/>
+      <c r="Z2" s="19"/>
+      <c r="AA2" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="W2" s="37"/>
-      <c r="X2" s="37"/>
-      <c r="Y2" s="38"/>
-      <c r="Z2" s="19"/>
-      <c r="AA2" s="36" t="s">
-        <v>8</v>
-      </c>
-      <c r="AB2" s="37"/>
-      <c r="AC2" s="37"/>
-      <c r="AD2" s="37"/>
-      <c r="AE2" s="37"/>
-      <c r="AF2" s="37"/>
-      <c r="AG2" s="38"/>
+      <c r="AB2" s="41"/>
+      <c r="AC2" s="41"/>
+      <c r="AD2" s="41"/>
+      <c r="AE2" s="41"/>
+      <c r="AF2" s="41"/>
+      <c r="AG2" s="42"/>
       <c r="AH2" s="20"/>
       <c r="AI2" s="22" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="AJ2" s="23"/>
       <c r="AK2" s="23"/>
@@ -1231,23 +2036,23 @@
       <c r="AP2" s="23"/>
     </row>
     <row r="3" spans="2:67" s="12" customFormat="1" ht="39.950000000000003" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="40" t="s">
+      <c r="B3" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="42" t="s">
+      <c r="C3" s="33" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="42" t="s">
+      <c r="E3" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="42" t="s">
+      <c r="F3" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="42" t="s">
+      <c r="G3" s="35" t="s">
         <v>14</v>
-      </c>
-      <c r="G3" s="30" t="s">
-        <v>15</v>
       </c>
       <c r="H3" s="21" t="s">
         <v>0</v>
@@ -1273,12 +2078,12 @@
       <c r="AA3" s="11"/>
     </row>
     <row r="4" spans="2:67" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="41"/>
-      <c r="C4" s="31"/>
-      <c r="D4" s="31"/>
-      <c r="E4" s="31"/>
-      <c r="F4" s="31"/>
-      <c r="G4" s="31"/>
+      <c r="B4" s="32"/>
+      <c r="C4" s="34"/>
+      <c r="D4" s="34"/>
+      <c r="E4" s="34"/>
+      <c r="F4" s="34"/>
+      <c r="G4" s="34"/>
       <c r="H4" s="3">
         <v>1</v>
       </c>
@@ -1462,7 +2267,7 @@
     </row>
     <row r="5" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="27" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C5" s="25"/>
       <c r="D5" s="25"/>
@@ -1472,7 +2277,7 @@
     </row>
     <row r="6" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="24" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C6" s="7">
         <v>1</v>
@@ -1492,7 +2297,7 @@
     </row>
     <row r="7" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="28" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C7" s="29"/>
       <c r="D7" s="29"/>
@@ -1502,7 +2307,7 @@
     </row>
     <row r="8" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="24" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C8" s="7">
         <v>4</v>
@@ -1522,7 +2327,7 @@
     </row>
     <row r="9" spans="2:67" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="24" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C9" s="7">
         <v>7</v>
@@ -1542,7 +2347,7 @@
     </row>
     <row r="10" spans="2:67" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="24" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C10" s="7">
         <v>11</v>
@@ -1562,7 +2367,7 @@
     </row>
     <row r="11" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="26" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C11" s="25"/>
       <c r="D11" s="25"/>
@@ -1572,7 +2377,7 @@
     </row>
     <row r="12" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="24" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C12" s="7">
         <v>14</v>
@@ -1592,7 +2397,7 @@
     </row>
     <row r="13" spans="2:67" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="28" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C13" s="29"/>
       <c r="D13" s="29"/>
@@ -1602,7 +2407,7 @@
     </row>
     <row r="14" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="24" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C14" s="7">
         <v>16</v>
@@ -1622,7 +2427,7 @@
     </row>
     <row r="15" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="24" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C15" s="9">
         <v>18</v>
@@ -1642,7 +2447,7 @@
     </row>
     <row r="16" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="24" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C16" s="7">
         <v>24</v>
@@ -1662,7 +2467,7 @@
     </row>
     <row r="17" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="28" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C17" s="29"/>
       <c r="D17" s="29"/>
@@ -1672,7 +2477,7 @@
     </row>
     <row r="18" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C18" s="7">
         <v>24</v>
@@ -1692,7 +2497,7 @@
     </row>
     <row r="19" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="24" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C19" s="7">
         <v>25</v>
@@ -1712,21 +2517,27 @@
     </row>
     <row r="20" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="24" t="s">
-        <v>41</v>
-      </c>
-      <c r="C20" s="7"/>
+        <v>40</v>
+      </c>
+      <c r="C20" s="7">
+        <v>28</v>
+      </c>
       <c r="D20" s="7">
         <v>28</v>
       </c>
-      <c r="E20" s="7"/>
-      <c r="F20" s="7"/>
+      <c r="E20" s="7">
+        <v>28</v>
+      </c>
+      <c r="F20" s="7">
+        <v>15</v>
+      </c>
       <c r="G20" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="26" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C21" s="25"/>
       <c r="D21" s="25"/>
@@ -1738,75 +2549,107 @@
     </row>
     <row r="22" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="C22" s="7">
         <v>43</v>
       </c>
-      <c r="C22" s="7"/>
       <c r="D22" s="7">
         <v>7</v>
       </c>
-      <c r="E22" s="7"/>
-      <c r="F22" s="7"/>
+      <c r="E22" s="7">
+        <v>44</v>
+      </c>
+      <c r="F22" s="7">
+        <v>3</v>
+      </c>
       <c r="G22" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B23" s="24" t="s">
-        <v>44</v>
-      </c>
-      <c r="C23" s="7"/>
+        <v>43</v>
+      </c>
+      <c r="C23" s="7">
+        <v>45</v>
+      </c>
       <c r="D23" s="7">
         <v>5</v>
       </c>
-      <c r="E23" s="7"/>
-      <c r="F23" s="7"/>
+      <c r="E23" s="7">
+        <v>46</v>
+      </c>
+      <c r="F23" s="7">
+        <v>1</v>
+      </c>
       <c r="G23" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="2:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="C24" s="7">
         <v>45</v>
       </c>
-      <c r="C24" s="7"/>
       <c r="D24" s="7">
         <v>5</v>
       </c>
-      <c r="E24" s="7"/>
-      <c r="F24" s="7"/>
+      <c r="E24" s="7">
+        <v>46</v>
+      </c>
+      <c r="F24" s="7">
+        <v>1</v>
+      </c>
       <c r="G24" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25" s="24" t="s">
-        <v>46</v>
-      </c>
-      <c r="C25" s="7"/>
+        <v>45</v>
+      </c>
+      <c r="C25" s="7">
+        <v>44</v>
+      </c>
       <c r="D25" s="7">
         <v>6</v>
       </c>
-      <c r="E25" s="7"/>
-      <c r="F25" s="7"/>
+      <c r="E25" s="7">
+        <v>44</v>
+      </c>
+      <c r="F25" s="7">
+        <v>2</v>
+      </c>
       <c r="G25" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="C26" s="7"/>
-      <c r="D26" s="7"/>
-      <c r="E26" s="7"/>
-      <c r="F26" s="7"/>
+      <c r="B26" s="24" t="s">
+        <v>49</v>
+      </c>
+      <c r="C26" s="7">
+        <v>49</v>
+      </c>
+      <c r="D26" s="7">
+        <v>1</v>
+      </c>
+      <c r="E26" s="7">
+        <v>49</v>
+      </c>
+      <c r="F26" s="7">
+        <v>1</v>
+      </c>
       <c r="G26" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B27" s="6" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C27" s="7"/>
       <c r="D27" s="7"/>
@@ -1818,7 +2661,7 @@
     </row>
     <row r="28" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B28" s="6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C28" s="7"/>
       <c r="D28" s="7"/>
@@ -1830,7 +2673,7 @@
     </row>
     <row r="29" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B29" s="6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C29" s="7"/>
       <c r="D29" s="7"/>
@@ -1842,7 +2685,7 @@
     </row>
     <row r="30" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B30" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C30" s="7"/>
       <c r="D30" s="7"/>
@@ -1854,7 +2697,7 @@
     </row>
     <row r="31" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B31" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C31" s="7"/>
       <c r="D31" s="7"/>
@@ -1866,7 +2709,7 @@
     </row>
     <row r="32" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B32" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C32" s="7"/>
       <c r="D32" s="7"/>
@@ -1878,7 +2721,7 @@
     </row>
     <row r="33" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B33" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C33" s="7"/>
       <c r="D33" s="7"/>
@@ -1890,7 +2733,7 @@
     </row>
     <row r="34" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B34" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C34" s="7"/>
       <c r="D34" s="7"/>
@@ -1902,7 +2745,7 @@
     </row>
     <row r="35" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B35" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C35" s="7"/>
       <c r="D35" s="7"/>
@@ -1914,7 +2757,7 @@
     </row>
     <row r="36" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B36" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C36" s="7"/>
       <c r="D36" s="7"/>
@@ -1926,7 +2769,7 @@
     </row>
     <row r="37" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B37" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C37" s="7"/>
       <c r="D37" s="7"/>
@@ -1938,7 +2781,7 @@
     </row>
     <row r="38" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B38" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C38" s="7"/>
       <c r="D38" s="7"/>
@@ -1950,7 +2793,7 @@
     </row>
     <row r="39" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B39" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C39" s="7"/>
       <c r="D39" s="7"/>
@@ -1962,17 +2805,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="G3:G4"/>
+    <mergeCell ref="K2:O2"/>
+    <mergeCell ref="Q2:T2"/>
+    <mergeCell ref="V2:Y2"/>
+    <mergeCell ref="AA2:AG2"/>
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="C3:C4"/>
     <mergeCell ref="D3:D4"/>
     <mergeCell ref="E3:E4"/>
     <mergeCell ref="F3:F4"/>
-    <mergeCell ref="G3:G4"/>
-    <mergeCell ref="K2:O2"/>
-    <mergeCell ref="Q2:T2"/>
-    <mergeCell ref="V2:Y2"/>
-    <mergeCell ref="AA2:AG2"/>
   </mergeCells>
   <phoneticPr fontId="14" type="noConversion"/>
   <conditionalFormatting sqref="H5:BO39">
@@ -2006,7 +2849,7 @@
       <formula>H$4=period_selected</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations disablePrompts="1" count="16">
+  <dataValidations count="16">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Project planner uses periods for intervals. Start=1 is period 1 and duration=5 means project spans 5 periods starting from start period. Enter data starting in B5 to update the chart" sqref="A1" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
     <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Type a value from 1 to 60 or select a period from the list-press  CANCEL, ALT+DOWN ARROW, then ENTER to select a value" prompt="Enter a period in the range of 1 to 60 or select a period from the list. Press ALT+DOWN ARROW to navigate the list, then ENTER to select a value" sqref="H2" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"1,2,3,4,5,6,7,8,9,10,11,12,13,14,15,16,17,18,19,20,21,22,23,24,25,26,27,28,29,30,31,32,33,34,35,36,37,38,39,40,41,42,43,44,45,46,47,48,49,50,51,52,53,54,55,56,57,58,59,60"</formula1>

</xml_diff>